<commit_message>
upd: teacher info in excel spreadsheet
</commit_message>
<xml_diff>
--- a/economic_game.xlsx
+++ b/economic_game.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>lastname</t>
   </si>
@@ -28,6 +28,12 @@
     <t>email</t>
   </si>
   <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>company_money</t>
+  </si>
+  <si>
     <t>Александров</t>
   </si>
   <si>
@@ -106,6 +112,60 @@
     <t>8А</t>
   </si>
   <si>
+    <t>Сагайдак</t>
+  </si>
+  <si>
+    <t>Полина</t>
+  </si>
+  <si>
+    <t>Тарасовна</t>
+  </si>
+  <si>
+    <t>12Б</t>
+  </si>
+  <si>
+    <t>polina.sagaidac@mail.ru</t>
+  </si>
+  <si>
+    <t>Илья</t>
+  </si>
+  <si>
+    <t>Тарасович</t>
+  </si>
+  <si>
+    <t>12А</t>
+  </si>
+  <si>
+    <t>m.s.v.inkognito@yandex.ru</t>
+  </si>
+  <si>
+    <t>Симошин</t>
+  </si>
+  <si>
+    <t>Михаил</t>
+  </si>
+  <si>
+    <t>Николаевич</t>
+  </si>
+  <si>
+    <t>9А</t>
+  </si>
+  <si>
+    <t>mih_z8@mail.ru</t>
+  </si>
+  <si>
+    <t>Васильева</t>
+  </si>
+  <si>
+    <t>Татьяна</t>
+  </si>
+  <si>
+    <t>Павловна</t>
+  </si>
+  <si>
+    <t>sdelorec@yandex.ru</t>
+  </si>
+  <si>
     <t>Валентинова</t>
   </si>
   <si>
@@ -115,6 +175,9 @@
     <t>Валентиновна</t>
   </si>
   <si>
+    <t>Кругосвет</t>
+  </si>
+  <si>
     <t>Игнатов</t>
   </si>
   <si>
@@ -124,58 +187,7 @@
     <t>Игнатьевич</t>
   </si>
   <si>
-    <t>Сагайдак</t>
-  </si>
-  <si>
-    <t>Полина</t>
-  </si>
-  <si>
-    <t>Тарасовна</t>
-  </si>
-  <si>
-    <t>12Б</t>
-  </si>
-  <si>
-    <t>polina.sagaidac@mail.ru</t>
-  </si>
-  <si>
-    <t>Симошин</t>
-  </si>
-  <si>
-    <t>Михаил</t>
-  </si>
-  <si>
-    <t>Николаевич</t>
-  </si>
-  <si>
-    <t>9А</t>
-  </si>
-  <si>
-    <t>mih_z8@mail.ru</t>
-  </si>
-  <si>
-    <t>Илья</t>
-  </si>
-  <si>
-    <t>Тарасович</t>
-  </si>
-  <si>
-    <t>12А</t>
-  </si>
-  <si>
-    <t>m.s.v.inkognito@yandex.ru</t>
-  </si>
-  <si>
-    <t>Васильева</t>
-  </si>
-  <si>
-    <t>Татьяна</t>
-  </si>
-  <si>
-    <t>Павловна</t>
-  </si>
-  <si>
-    <t>sdelorec@yandex.ru</t>
+    <t>Цифромир</t>
   </si>
 </sst>
 </file>
@@ -448,193 +460,211 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1000.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="1">
+        <v>2000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>